<commit_message>
Transacao - Implentação da rota de cadastro por planilha - conclusão * controller - inclusão método * DTOs - de retorno com os dados da importação da planilha * service - criação método principal
Diversos
* Script SQL - ajuste da view que inclui o saldo a transação
* classes auxiliares a implemntação da imoprtação de transação por planilha
* Inclusão de handlers no Tratador de Erros central
* Atualização Readme
* Atualização da collection Postman
</commit_message>
<xml_diff>
--- a/arquivos/transacoes-importacao-2025-02-teste.xlsx
+++ b/arquivos/transacoes-importacao-2025-02-teste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_java\gestaofinanceira\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1205562-D7DB-43E0-AA06-70DCEDE75736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC668073-22CC-46E2-B8C1-F1403D3F5E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{575A127D-61A6-4E18-8B2F-1C1003BBD3E8}"/>
   </bookViews>
@@ -16,11 +16,11 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,59 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Marcelo Silva Santos</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{267AA4A2-D43F-4429-9FB5-38444FA2C499}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">"NULL" = ainda não foi importado
-"SIM" = foi importado
-"NÂO" = Houve algum problema ao tentar importar (veja coluna MOTIVO)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{83C63443-3117-4E0E-B706-30B69C3C39BB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Preenchido com o motivo de não poder ser importado
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>RECEITA</t>
   </si>
@@ -128,24 +77,12 @@
     <t>regular</t>
   </si>
   <si>
-    <t>DIA</t>
-  </si>
-  <si>
-    <t>IMPORTADO</t>
-  </si>
-  <si>
-    <t>MOTIVO</t>
-  </si>
-  <si>
     <t>MÉTODO</t>
   </si>
   <si>
     <t>TIPO DE TRANSACAO</t>
   </si>
   <si>
-    <t>Riocard</t>
-  </si>
-  <si>
     <t>XXX</t>
   </si>
   <si>
@@ -155,29 +92,31 @@
     <t>ZZZ</t>
   </si>
   <si>
-    <t>SIM</t>
-  </si>
-  <si>
-    <t>NÃO</t>
-  </si>
-  <si>
-    <t>[CATEGORIA]: A 'categoria' não pode ser 'null' ou 'vazio'
-[MÉTODO]: O 'método' passado 'ZZZ' não é valido, é esperado '[TRANSFERENCIA, OUTRO_METODO_DE_RECEITA, CARTAO_CREDITO, CARTAO_DEBITO, PIX, OUTRO_METODO_DE_DESPESA]'.</t>
-  </si>
-  <si>
-    <t>[TIPO]: O 'tipo' passado 'XXX' não é valido, é esperado '[RECEITA, DESPESA]'.
-[CATEGORIA]: A 'categoria' passada 'YYY' não é valida, é esperado '[SALARIO, PROVENTOS, OUTRA_CATEGORIA_DE_RECEITA, ALIMENTACAO, PASSEIO, TRANSPORTE, EDUCACAO, OUTRA_CATEGORIA_DE_DESPESA]'.</t>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Riocard - XXX</t>
+  </si>
+  <si>
+    <t>Data e Hora</t>
+  </si>
+  <si>
+    <t>ALIMENTACAO</t>
+  </si>
+  <si>
+    <t>CARTAO_DEBITO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,19 +140,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,23 +196,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -290,29 +216,56 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -648,181 +601,307 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9708B0-8338-4D39-8FB4-212B6F5F1CC4}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9708B0-8338-4D39-8FB4-212B6F5F1CC4}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="10.08984375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="28.6328125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="27.26953125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="12.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="15.6328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="26.7265625"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="15.453125"/>
-    <col min="8" max="8" customWidth="true" style="6" width="200.6328125"/>
-    <col min="9" max="16384" style="4" width="8.7265625"/>
+    <col min="1" max="1" width="21.7265625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>45689.416678240741</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14">
+        <v>12318.45</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
+        <v>45691.005578703705</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="22">
+        <v>-368.4</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>45693.000034722223</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="14">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19">
+        <v>45693.458379629628</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="C5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1800</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10">
-        <v>45689</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="F5" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="22">
+        <v>650</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>45689.41673611111</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D7" s="14">
         <v>12318.45</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="s">
+    </row>
+    <row r="8" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19">
+        <v>45691.005636574075</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="22">
+        <v>-368.4</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>45693.000671296293</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2500</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>45693.000810185185</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>45701.381377314814</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14">
+        <v>-185</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
-        <v>45691</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="13">
-        <v>368.4</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10">
-        <v>45693</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    </row>
+    <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>45714</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="14">
         <v>0</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="E12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>45693</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1800</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
-        <v>45693</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="13">
-        <v>650</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="9"/>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H6" xr:uid="{6E9708B0-8338-4D39-8FB4-212B6F5F1CC4}"/>
+  <autoFilter ref="A1:F6" xr:uid="{6E9708B0-8338-4D39-8FB4-212B6F5F1CC4}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>